<commit_message>
initial profiles and examples
</commit_message>
<xml_diff>
--- a/public/StructureDefinition-MyPatient.xlsx
+++ b/public/StructureDefinition-MyPatient.xlsx
@@ -9,9 +9,6 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$46</definedName>
-  </definedNames>
 </workbook>
 </file>
 
@@ -57,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-01-06T20:47:49-06:00</t>
+    <t>2022-01-16T18:37:33-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1278,21 +1275,6 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color indexed="22"/>
-        <i val="true"/>
-      </font>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -1632,7 +1614,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" hidden="true">
+    <row r="2">
       <c r="A2" t="s" s="2">
         <v>27</v>
       </c>
@@ -1744,7 +1726,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" hidden="true">
+    <row r="3">
       <c r="A3" t="s" s="2">
         <v>83</v>
       </c>
@@ -1858,7 +1840,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" hidden="true">
+    <row r="4">
       <c r="A4" t="s" s="2">
         <v>91</v>
       </c>
@@ -1970,7 +1952,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" hidden="true">
+    <row r="5">
       <c r="A5" t="s" s="2">
         <v>97</v>
       </c>
@@ -2084,7 +2066,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" hidden="true">
+    <row r="6">
       <c r="A6" t="s" s="2">
         <v>103</v>
       </c>
@@ -2198,7 +2180,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" hidden="true">
+    <row r="7">
       <c r="A7" t="s" s="2">
         <v>112</v>
       </c>
@@ -2312,7 +2294,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" hidden="true">
+    <row r="8">
       <c r="A8" t="s" s="2">
         <v>120</v>
       </c>
@@ -2426,7 +2408,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" hidden="true">
+    <row r="9">
       <c r="A9" t="s" s="2">
         <v>128</v>
       </c>
@@ -2540,7 +2522,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" hidden="true">
+    <row r="10">
       <c r="A10" t="s" s="2">
         <v>136</v>
       </c>
@@ -2656,7 +2638,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
         <v>141</v>
       </c>
@@ -2770,7 +2752,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" hidden="true">
+    <row r="12">
       <c r="A12" t="s" s="2">
         <v>150</v>
       </c>
@@ -2898,13 +2880,13 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F13" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>77</v>
@@ -3004,7 +2986,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" hidden="true">
+    <row r="14">
       <c r="A14" t="s" s="2">
         <v>169</v>
       </c>
@@ -3120,7 +3102,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" hidden="true">
+    <row r="15">
       <c r="A15" t="s" s="2">
         <v>178</v>
       </c>
@@ -3236,7 +3218,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
         <v>189</v>
       </c>
@@ -3352,7 +3334,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>199</v>
       </c>
@@ -3468,7 +3450,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" hidden="true">
+    <row r="18">
       <c r="A18" t="s" s="2">
         <v>207</v>
       </c>
@@ -3584,7 +3566,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
         <v>216</v>
       </c>
@@ -3698,7 +3680,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
         <v>227</v>
       </c>
@@ -3814,7 +3796,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
         <v>235</v>
       </c>
@@ -3930,7 +3912,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
         <v>243</v>
       </c>
@@ -4046,7 +4028,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
         <v>251</v>
       </c>
@@ -4158,7 +4140,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" hidden="true">
+    <row r="24">
       <c r="A24" t="s" s="2">
         <v>255</v>
       </c>
@@ -4272,7 +4254,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" hidden="true">
+    <row r="25">
       <c r="A25" t="s" s="2">
         <v>258</v>
       </c>
@@ -4388,7 +4370,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
         <v>263</v>
       </c>
@@ -4502,7 +4484,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" hidden="true">
+    <row r="27">
       <c r="A27" t="s" s="2">
         <v>271</v>
       </c>
@@ -4616,7 +4598,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" hidden="true">
+    <row r="28">
       <c r="A28" t="s" s="2">
         <v>276</v>
       </c>
@@ -4732,7 +4714,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" hidden="true">
+    <row r="29">
       <c r="A29" t="s" s="2">
         <v>281</v>
       </c>
@@ -4846,7 +4828,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
         <v>286</v>
       </c>
@@ -4960,7 +4942,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" hidden="true">
+    <row r="31">
       <c r="A31" t="s" s="2">
         <v>290</v>
       </c>
@@ -5074,7 +5056,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
         <v>298</v>
       </c>
@@ -5186,7 +5168,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" hidden="true">
+    <row r="33">
       <c r="A33" t="s" s="2">
         <v>303</v>
       </c>
@@ -5302,7 +5284,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" hidden="true">
+    <row r="34">
       <c r="A34" t="s" s="2">
         <v>310</v>
       </c>
@@ -5414,7 +5396,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
         <v>311</v>
       </c>
@@ -5528,7 +5510,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" hidden="true">
+    <row r="36">
       <c r="A36" t="s" s="2">
         <v>312</v>
       </c>
@@ -5644,7 +5626,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" hidden="true">
+    <row r="37">
       <c r="A37" t="s" s="2">
         <v>313</v>
       </c>
@@ -5760,7 +5742,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
         <v>321</v>
       </c>
@@ -5876,7 +5858,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" hidden="true">
+    <row r="39">
       <c r="A39" t="s" s="2">
         <v>329</v>
       </c>
@@ -5990,7 +5972,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" hidden="true">
+    <row r="40">
       <c r="A40" t="s" s="2">
         <v>337</v>
       </c>
@@ -6106,7 +6088,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" hidden="true">
+    <row r="41">
       <c r="A41" t="s" s="2">
         <v>343</v>
       </c>
@@ -6222,7 +6204,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" hidden="true">
+    <row r="42">
       <c r="A42" t="s" s="2">
         <v>349</v>
       </c>
@@ -6334,7 +6316,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" hidden="true">
+    <row r="43">
       <c r="A43" t="s" s="2">
         <v>350</v>
       </c>
@@ -6448,7 +6430,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" hidden="true">
+    <row r="44">
       <c r="A44" t="s" s="2">
         <v>351</v>
       </c>
@@ -6564,7 +6546,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" hidden="true">
+    <row r="45">
       <c r="A45" t="s" s="2">
         <v>352</v>
       </c>
@@ -6678,7 +6660,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" hidden="true">
+    <row r="46">
       <c r="A46" t="s" s="2">
         <v>358</v>
       </c>
@@ -6791,24 +6773,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN46">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="26">
-      <filters blank="true"/>
-    </filterColumn>
-  </autoFilter>
-  <conditionalFormatting sqref="A2:AI45">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$G2&lt;&gt;"Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$Q2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>